<commit_message>
Updated script to modify result Excel in amazon-seller-data-analysis
</commit_message>
<xml_diff>
--- a/Amazon-Seller-Data-Analysis/cleaned_orders.xlsx
+++ b/Amazon-Seller-Data-Analysis/cleaned_orders.xlsx
@@ -561,10 +561,8 @@
       <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
+      <c r="I2" t="n">
+        <v>449</v>
       </c>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
@@ -634,15 +632,11 @@
       <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I3" t="n">
+        <v>449</v>
+      </c>
+      <c r="J3" t="n">
+        <v>60.18</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr">
@@ -711,15 +705,11 @@
       <c r="H4" t="n">
         <v>1</v>
       </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I4" t="n">
+        <v>449</v>
+      </c>
+      <c r="J4" t="n">
+        <v>60.18</v>
       </c>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
@@ -861,15 +851,11 @@
       <c r="H6" t="n">
         <v>1</v>
       </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I6" t="n">
+        <v>1099</v>
+      </c>
+      <c r="J6" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
@@ -938,10 +924,8 @@
       <c r="H7" t="n">
         <v>1</v>
       </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>200.00</t>
-        </is>
+      <c r="I7" t="n">
+        <v>200</v>
       </c>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
@@ -1084,15 +1068,11 @@
       <c r="H9" t="n">
         <v>1</v>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I9" t="n">
+        <v>399</v>
+      </c>
+      <c r="J9" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1165,15 +1145,11 @@
       <c r="H10" t="n">
         <v>1</v>
       </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I10" t="n">
+        <v>399</v>
+      </c>
+      <c r="J10" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr">
@@ -1242,10 +1218,8 @@
       <c r="H11" t="n">
         <v>1</v>
       </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
+      <c r="I11" t="n">
+        <v>1099</v>
       </c>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
@@ -1315,15 +1289,11 @@
       <c r="H12" t="n">
         <v>1</v>
       </c>
-      <c r="I12" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>114.46</t>
-        </is>
+      <c r="I12" t="n">
+        <v>449</v>
+      </c>
+      <c r="J12" t="n">
+        <v>114.46</v>
       </c>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr">
@@ -1392,15 +1362,11 @@
       <c r="H13" t="n">
         <v>1</v>
       </c>
-      <c r="I13" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I13" t="n">
+        <v>449</v>
+      </c>
+      <c r="J13" t="n">
+        <v>60.18</v>
       </c>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr">
@@ -1469,15 +1435,11 @@
       <c r="H14" t="n">
         <v>1</v>
       </c>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I14" t="n">
+        <v>449</v>
+      </c>
+      <c r="J14" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1550,15 +1512,11 @@
       <c r="H15" t="n">
         <v>1</v>
       </c>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I15" t="n">
+        <v>1099</v>
+      </c>
+      <c r="J15" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr">
@@ -1628,10 +1586,8 @@
         <v>1</v>
       </c>
       <c r="I16" t="inlineStr"/>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J16" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1704,15 +1660,11 @@
       <c r="H17" t="n">
         <v>1</v>
       </c>
-      <c r="I17" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>62.54</t>
-        </is>
+      <c r="I17" t="n">
+        <v>1099</v>
+      </c>
+      <c r="J17" t="n">
+        <v>62.54</v>
       </c>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr">
@@ -1781,15 +1733,11 @@
       <c r="H18" t="n">
         <v>1</v>
       </c>
-      <c r="I18" t="inlineStr">
-        <is>
-          <t>649.00</t>
-        </is>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>81.42</t>
-        </is>
+      <c r="I18" t="n">
+        <v>649</v>
+      </c>
+      <c r="J18" t="n">
+        <v>81.42</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
@@ -1862,15 +1810,11 @@
       <c r="H19" t="n">
         <v>1</v>
       </c>
-      <c r="I19" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I19" t="n">
+        <v>449</v>
+      </c>
+      <c r="J19" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr">
@@ -1939,15 +1883,11 @@
       <c r="H20" t="n">
         <v>1</v>
       </c>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I20" t="n">
+        <v>399</v>
+      </c>
+      <c r="J20" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr">
@@ -2016,15 +1956,11 @@
       <c r="H21" t="n">
         <v>1</v>
       </c>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I21" t="n">
+        <v>399</v>
+      </c>
+      <c r="J21" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K21" t="inlineStr">
         <is>
@@ -2097,15 +2033,11 @@
       <c r="H22" t="n">
         <v>1</v>
       </c>
-      <c r="I22" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I22" t="n">
+        <v>399</v>
+      </c>
+      <c r="J22" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr">
@@ -2174,15 +2106,11 @@
       <c r="H23" t="n">
         <v>1</v>
       </c>
-      <c r="I23" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I23" t="n">
+        <v>449</v>
+      </c>
+      <c r="J23" t="n">
+        <v>60.18</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr">
@@ -2252,10 +2180,8 @@
         <v>1</v>
       </c>
       <c r="I24" t="inlineStr"/>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J24" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K24" t="inlineStr"/>
       <c r="L24" t="inlineStr">
@@ -2324,15 +2250,11 @@
       <c r="H25" t="n">
         <v>1</v>
       </c>
-      <c r="I25" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I25" t="n">
+        <v>399</v>
+      </c>
+      <c r="J25" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr">
@@ -2474,15 +2396,11 @@
       <c r="H27" t="n">
         <v>1</v>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>649.00</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I27" t="n">
+        <v>649</v>
+      </c>
+      <c r="J27" t="n">
+        <v>60.18</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
@@ -2555,10 +2473,8 @@
       <c r="H28" t="n">
         <v>1</v>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
+      <c r="I28" t="n">
+        <v>250</v>
       </c>
       <c r="J28" t="inlineStr"/>
       <c r="K28" t="inlineStr"/>
@@ -2628,15 +2544,11 @@
       <c r="H29" t="n">
         <v>1</v>
       </c>
-      <c r="I29" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I29" t="n">
+        <v>449</v>
+      </c>
+      <c r="J29" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
@@ -2709,15 +2621,11 @@
       <c r="H30" t="n">
         <v>1</v>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I30" t="n">
+        <v>399</v>
+      </c>
+      <c r="J30" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
@@ -2790,10 +2698,8 @@
       <c r="H31" t="n">
         <v>1</v>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
+      <c r="I31" t="n">
+        <v>449</v>
       </c>
       <c r="J31" t="inlineStr"/>
       <c r="K31" t="inlineStr"/>
@@ -2863,15 +2769,11 @@
       <c r="H32" t="n">
         <v>1</v>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I32" t="n">
+        <v>449</v>
+      </c>
+      <c r="J32" t="n">
+        <v>60.18</v>
       </c>
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr">
@@ -2940,15 +2842,11 @@
       <c r="H33" t="n">
         <v>1</v>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I33" t="n">
+        <v>399</v>
+      </c>
+      <c r="J33" t="n">
+        <v>60.18</v>
       </c>
       <c r="K33" t="inlineStr"/>
       <c r="L33" t="inlineStr">
@@ -3017,15 +2915,11 @@
       <c r="H34" t="n">
         <v>1</v>
       </c>
-      <c r="I34" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I34" t="n">
+        <v>449</v>
+      </c>
+      <c r="J34" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
@@ -3098,15 +2992,11 @@
       <c r="H35" t="n">
         <v>1</v>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I35" t="n">
+        <v>449</v>
+      </c>
+      <c r="J35" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr">
@@ -3175,15 +3065,11 @@
       <c r="H36" t="n">
         <v>1</v>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I36" t="n">
+        <v>250</v>
+      </c>
+      <c r="J36" t="n">
+        <v>47.2</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
@@ -3256,15 +3142,11 @@
       <c r="H37" t="n">
         <v>1</v>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I37" t="n">
+        <v>399</v>
+      </c>
+      <c r="J37" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K37" t="inlineStr"/>
       <c r="L37" t="inlineStr">
@@ -3333,15 +3215,11 @@
       <c r="H38" t="n">
         <v>1</v>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I38" t="n">
+        <v>399</v>
+      </c>
+      <c r="J38" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr">
@@ -3410,15 +3288,11 @@
       <c r="H39" t="n">
         <v>1</v>
       </c>
-      <c r="I39" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I39" t="n">
+        <v>449</v>
+      </c>
+      <c r="J39" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K39" t="inlineStr"/>
       <c r="L39" t="inlineStr">
@@ -3487,15 +3361,11 @@
       <c r="H40" t="n">
         <v>1</v>
       </c>
-      <c r="I40" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I40" t="n">
+        <v>399</v>
+      </c>
+      <c r="J40" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K40" t="inlineStr">
         <is>
@@ -3569,10 +3439,8 @@
         <v>4</v>
       </c>
       <c r="I41" t="inlineStr"/>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J41" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr">
@@ -3641,15 +3509,11 @@
       <c r="H42" t="n">
         <v>1</v>
       </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I42" t="n">
+        <v>549</v>
+      </c>
+      <c r="J42" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K42" t="inlineStr"/>
       <c r="L42" t="inlineStr">
@@ -3718,15 +3582,11 @@
       <c r="H43" t="n">
         <v>1</v>
       </c>
-      <c r="I43" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I43" t="n">
+        <v>250</v>
+      </c>
+      <c r="J43" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr">
@@ -3795,15 +3655,11 @@
       <c r="H44" t="n">
         <v>1</v>
       </c>
-      <c r="I44" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I44" t="n">
+        <v>449</v>
+      </c>
+      <c r="J44" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K44" t="inlineStr"/>
       <c r="L44" t="inlineStr">
@@ -3873,10 +3729,8 @@
         <v>1</v>
       </c>
       <c r="I45" t="inlineStr"/>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="J45" t="n">
+        <v>47.2</v>
       </c>
       <c r="K45" t="inlineStr"/>
       <c r="L45" t="inlineStr">
@@ -3945,10 +3799,8 @@
       <c r="H46" t="n">
         <v>1</v>
       </c>
-      <c r="I46" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
+      <c r="I46" t="n">
+        <v>449</v>
       </c>
       <c r="J46" t="inlineStr"/>
       <c r="K46" t="inlineStr"/>
@@ -4018,15 +3870,11 @@
       <c r="H47" t="n">
         <v>1</v>
       </c>
-      <c r="I47" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I47" t="n">
+        <v>250</v>
+      </c>
+      <c r="J47" t="n">
+        <v>60.18</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
@@ -4099,10 +3947,8 @@
       <c r="H48" t="n">
         <v>1</v>
       </c>
-      <c r="I48" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
+      <c r="I48" t="n">
+        <v>1099</v>
       </c>
       <c r="J48" t="inlineStr"/>
       <c r="K48" t="inlineStr">
@@ -4177,10 +4023,8 @@
         <v>1</v>
       </c>
       <c r="I49" t="inlineStr"/>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="J49" t="n">
+        <v>60.18</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
@@ -4253,10 +4097,8 @@
       <c r="H50" t="n">
         <v>1</v>
       </c>
-      <c r="I50" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
+      <c r="I50" t="n">
+        <v>1099</v>
       </c>
       <c r="J50" t="inlineStr"/>
       <c r="K50" t="inlineStr">
@@ -4330,15 +4172,11 @@
       <c r="H51" t="n">
         <v>1</v>
       </c>
-      <c r="I51" t="inlineStr">
-        <is>
-          <t>649.00</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I51" t="n">
+        <v>649</v>
+      </c>
+      <c r="J51" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr">
@@ -4407,15 +4245,11 @@
       <c r="H52" t="n">
         <v>1</v>
       </c>
-      <c r="I52" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I52" t="n">
+        <v>449</v>
+      </c>
+      <c r="J52" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
@@ -4488,10 +4322,8 @@
       <c r="H53" t="n">
         <v>1</v>
       </c>
-      <c r="I53" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
+      <c r="I53" t="n">
+        <v>399</v>
       </c>
       <c r="J53" t="inlineStr"/>
       <c r="K53" t="inlineStr"/>
@@ -4561,10 +4393,8 @@
       <c r="H54" t="n">
         <v>1</v>
       </c>
-      <c r="I54" t="inlineStr">
-        <is>
-          <t>175.00</t>
-        </is>
+      <c r="I54" t="n">
+        <v>175</v>
       </c>
       <c r="J54" t="inlineStr"/>
       <c r="K54" t="inlineStr">
@@ -4638,15 +4468,11 @@
       <c r="H55" t="n">
         <v>1</v>
       </c>
-      <c r="I55" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I55" t="n">
+        <v>449</v>
+      </c>
+      <c r="J55" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
@@ -4719,15 +4545,11 @@
       <c r="H56" t="n">
         <v>1</v>
       </c>
-      <c r="I56" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I56" t="n">
+        <v>549</v>
+      </c>
+      <c r="J56" t="n">
+        <v>47.2</v>
       </c>
       <c r="K56" t="inlineStr"/>
       <c r="L56" t="inlineStr">
@@ -4796,15 +4618,11 @@
       <c r="H57" t="n">
         <v>1</v>
       </c>
-      <c r="I57" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I57" t="n">
+        <v>399</v>
+      </c>
+      <c r="J57" t="n">
+        <v>47.2</v>
       </c>
       <c r="K57" t="inlineStr"/>
       <c r="L57" t="inlineStr">
@@ -4873,10 +4691,8 @@
       <c r="H58" t="n">
         <v>1</v>
       </c>
-      <c r="I58" t="inlineStr">
-        <is>
-          <t>175.00</t>
-        </is>
+      <c r="I58" t="n">
+        <v>175</v>
       </c>
       <c r="J58" t="inlineStr"/>
       <c r="K58" t="inlineStr"/>
@@ -4946,15 +4762,11 @@
       <c r="H59" t="n">
         <v>1</v>
       </c>
-      <c r="I59" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I59" t="n">
+        <v>399</v>
+      </c>
+      <c r="J59" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K59" t="inlineStr"/>
       <c r="L59" t="inlineStr">
@@ -5023,15 +4835,11 @@
       <c r="H60" t="n">
         <v>1</v>
       </c>
-      <c r="I60" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>178.18</t>
-        </is>
+      <c r="I60" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J60" t="n">
+        <v>178.18</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
@@ -5104,10 +4912,8 @@
       <c r="H61" t="n">
         <v>1</v>
       </c>
-      <c r="I61" t="inlineStr">
-        <is>
-          <t>175.00</t>
-        </is>
+      <c r="I61" t="n">
+        <v>175</v>
       </c>
       <c r="J61" t="inlineStr"/>
       <c r="K61" t="inlineStr"/>
@@ -5177,10 +4983,8 @@
       <c r="H62" t="n">
         <v>1</v>
       </c>
-      <c r="I62" t="inlineStr">
-        <is>
-          <t>175.00</t>
-        </is>
+      <c r="I62" t="n">
+        <v>175</v>
       </c>
       <c r="J62" t="inlineStr"/>
       <c r="K62" t="inlineStr"/>
@@ -5250,15 +5054,11 @@
       <c r="H63" t="n">
         <v>1</v>
       </c>
-      <c r="I63" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I63" t="n">
+        <v>399</v>
+      </c>
+      <c r="J63" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K63" t="inlineStr"/>
       <c r="L63" t="inlineStr">
@@ -5327,15 +5127,11 @@
       <c r="H64" t="n">
         <v>1</v>
       </c>
-      <c r="I64" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I64" t="n">
+        <v>399</v>
+      </c>
+      <c r="J64" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K64" t="inlineStr"/>
       <c r="L64" t="inlineStr">
@@ -5404,10 +5200,8 @@
       <c r="H65" t="n">
         <v>1</v>
       </c>
-      <c r="I65" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
+      <c r="I65" t="n">
+        <v>349</v>
       </c>
       <c r="J65" t="inlineStr"/>
       <c r="K65" t="inlineStr"/>
@@ -5478,10 +5272,8 @@
         <v>1</v>
       </c>
       <c r="I66" t="inlineStr"/>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J66" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K66" t="inlineStr"/>
       <c r="L66" t="inlineStr">
@@ -5550,15 +5342,11 @@
       <c r="H67" t="n">
         <v>1</v>
       </c>
-      <c r="I67" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I67" t="n">
+        <v>449</v>
+      </c>
+      <c r="J67" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K67" t="inlineStr"/>
       <c r="L67" t="inlineStr">
@@ -5627,15 +5415,11 @@
       <c r="H68" t="n">
         <v>1</v>
       </c>
-      <c r="I68" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I68" t="n">
+        <v>399</v>
+      </c>
+      <c r="J68" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
@@ -5708,15 +5492,11 @@
       <c r="H69" t="n">
         <v>1</v>
       </c>
-      <c r="I69" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I69" t="n">
+        <v>449</v>
+      </c>
+      <c r="J69" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K69" t="inlineStr"/>
       <c r="L69" t="inlineStr">
@@ -5785,10 +5565,8 @@
       <c r="H70" t="n">
         <v>1</v>
       </c>
-      <c r="I70" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
+      <c r="I70" t="n">
+        <v>449</v>
       </c>
       <c r="J70" t="inlineStr"/>
       <c r="K70" t="inlineStr"/>
@@ -5858,15 +5636,11 @@
       <c r="H71" t="n">
         <v>1</v>
       </c>
-      <c r="I71" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I71" t="n">
+        <v>449</v>
+      </c>
+      <c r="J71" t="n">
+        <v>47.2</v>
       </c>
       <c r="K71" t="inlineStr"/>
       <c r="L71" t="inlineStr">
@@ -5935,15 +5709,11 @@
       <c r="H72" t="n">
         <v>1</v>
       </c>
-      <c r="I72" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I72" t="n">
+        <v>399</v>
+      </c>
+      <c r="J72" t="n">
+        <v>60.18</v>
       </c>
       <c r="K72" t="inlineStr"/>
       <c r="L72" t="inlineStr">
@@ -6012,10 +5782,8 @@
       <c r="H73" t="n">
         <v>1</v>
       </c>
-      <c r="I73" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
+      <c r="I73" t="n">
+        <v>250</v>
       </c>
       <c r="J73" t="inlineStr"/>
       <c r="K73" t="inlineStr"/>
@@ -6085,10 +5853,8 @@
       <c r="H74" t="n">
         <v>1</v>
       </c>
-      <c r="I74" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
+      <c r="I74" t="n">
+        <v>349</v>
       </c>
       <c r="J74" t="inlineStr"/>
       <c r="K74" t="inlineStr"/>
@@ -6158,10 +5924,8 @@
       <c r="H75" t="n">
         <v>1</v>
       </c>
-      <c r="I75" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
+      <c r="I75" t="n">
+        <v>549</v>
       </c>
       <c r="J75" t="inlineStr"/>
       <c r="K75" t="inlineStr">
@@ -6235,15 +5999,11 @@
       <c r="H76" t="n">
         <v>1</v>
       </c>
-      <c r="I76" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>210.04</t>
-        </is>
+      <c r="I76" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J76" t="n">
+        <v>210.04</v>
       </c>
       <c r="K76" t="inlineStr"/>
       <c r="L76" t="inlineStr">
@@ -6312,15 +6072,11 @@
       <c r="H77" t="n">
         <v>1</v>
       </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J77" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I77" t="n">
+        <v>449</v>
+      </c>
+      <c r="J77" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K77" t="inlineStr"/>
       <c r="L77" t="inlineStr">
@@ -6389,10 +6145,8 @@
       <c r="H78" t="n">
         <v>1</v>
       </c>
-      <c r="I78" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
+      <c r="I78" t="n">
+        <v>349</v>
       </c>
       <c r="J78" t="inlineStr"/>
       <c r="K78" t="inlineStr">
@@ -6466,15 +6220,11 @@
       <c r="H79" t="n">
         <v>1</v>
       </c>
-      <c r="I79" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I79" t="n">
+        <v>250</v>
+      </c>
+      <c r="J79" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K79" t="inlineStr">
         <is>
@@ -6547,15 +6297,11 @@
       <c r="H80" t="n">
         <v>1</v>
       </c>
-      <c r="I80" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I80" t="n">
+        <v>449</v>
+      </c>
+      <c r="J80" t="n">
+        <v>60.18</v>
       </c>
       <c r="K80" t="inlineStr"/>
       <c r="L80" t="inlineStr">
@@ -6624,15 +6370,11 @@
       <c r="H81" t="n">
         <v>1</v>
       </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I81" t="n">
+        <v>549</v>
+      </c>
+      <c r="J81" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K81" t="inlineStr"/>
       <c r="L81" t="inlineStr">
@@ -6701,15 +6443,11 @@
       <c r="H82" t="n">
         <v>1</v>
       </c>
-      <c r="I82" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I82" t="n">
+        <v>399</v>
+      </c>
+      <c r="J82" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K82" t="inlineStr"/>
       <c r="L82" t="inlineStr">
@@ -6778,15 +6516,11 @@
       <c r="H83" t="n">
         <v>1</v>
       </c>
-      <c r="I83" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I83" t="n">
+        <v>399</v>
+      </c>
+      <c r="J83" t="n">
+        <v>47.2</v>
       </c>
       <c r="K83" t="inlineStr"/>
       <c r="L83" t="inlineStr">
@@ -6855,15 +6589,11 @@
       <c r="H84" t="n">
         <v>1</v>
       </c>
-      <c r="I84" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I84" t="n">
+        <v>399</v>
+      </c>
+      <c r="J84" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K84" t="inlineStr"/>
       <c r="L84" t="inlineStr">
@@ -6932,15 +6662,11 @@
       <c r="H85" t="n">
         <v>1</v>
       </c>
-      <c r="I85" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>114.46</t>
-        </is>
+      <c r="I85" t="n">
+        <v>549</v>
+      </c>
+      <c r="J85" t="n">
+        <v>114.46</v>
       </c>
       <c r="K85" t="inlineStr"/>
       <c r="L85" t="inlineStr">
@@ -7009,15 +6735,11 @@
       <c r="H86" t="n">
         <v>1</v>
       </c>
-      <c r="I86" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I86" t="n">
+        <v>449</v>
+      </c>
+      <c r="J86" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K86" t="inlineStr"/>
       <c r="L86" t="inlineStr">
@@ -7086,15 +6808,11 @@
       <c r="H87" t="n">
         <v>1</v>
       </c>
-      <c r="I87" t="inlineStr">
-        <is>
-          <t>250.00</t>
-        </is>
-      </c>
-      <c r="J87" t="inlineStr">
-        <is>
-          <t>81.42</t>
-        </is>
+      <c r="I87" t="n">
+        <v>250</v>
+      </c>
+      <c r="J87" t="n">
+        <v>81.42</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
@@ -7167,15 +6885,11 @@
       <c r="H88" t="n">
         <v>2</v>
       </c>
-      <c r="I88" t="inlineStr">
-        <is>
-          <t>898.00</t>
-        </is>
-      </c>
-      <c r="J88" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I88" t="n">
+        <v>898</v>
+      </c>
+      <c r="J88" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K88" t="inlineStr"/>
       <c r="L88" t="inlineStr">
@@ -7245,10 +6959,8 @@
         <v>1</v>
       </c>
       <c r="I89" t="inlineStr"/>
-      <c r="J89" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J89" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K89" t="inlineStr"/>
       <c r="L89" t="inlineStr">
@@ -7317,15 +7029,11 @@
       <c r="H90" t="n">
         <v>1</v>
       </c>
-      <c r="I90" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J90" t="inlineStr">
-        <is>
-          <t>210.04</t>
-        </is>
+      <c r="I90" t="n">
+        <v>399</v>
+      </c>
+      <c r="J90" t="n">
+        <v>210.04</v>
       </c>
       <c r="K90" t="inlineStr"/>
       <c r="L90" t="inlineStr">
@@ -7394,10 +7102,8 @@
       <c r="H91" t="n">
         <v>1</v>
       </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
+      <c r="I91" t="n">
+        <v>449</v>
       </c>
       <c r="J91" t="inlineStr"/>
       <c r="K91" t="inlineStr"/>
@@ -7467,10 +7173,8 @@
       <c r="H92" t="n">
         <v>1</v>
       </c>
-      <c r="I92" t="inlineStr">
-        <is>
-          <t>1,099.00</t>
-        </is>
+      <c r="I92" t="n">
+        <v>1099</v>
       </c>
       <c r="J92" t="inlineStr"/>
       <c r="K92" t="inlineStr">
@@ -7544,15 +7248,11 @@
       <c r="H93" t="n">
         <v>1</v>
       </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J93" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I93" t="n">
+        <v>399</v>
+      </c>
+      <c r="J93" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K93" t="inlineStr"/>
       <c r="L93" t="inlineStr">
@@ -7621,15 +7321,11 @@
       <c r="H94" t="n">
         <v>1</v>
       </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>649.00</t>
-        </is>
-      </c>
-      <c r="J94" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I94" t="n">
+        <v>649</v>
+      </c>
+      <c r="J94" t="n">
+        <v>60.18</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
@@ -7702,10 +7398,8 @@
       <c r="H95" t="n">
         <v>1</v>
       </c>
-      <c r="I95" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
+      <c r="I95" t="n">
+        <v>399</v>
       </c>
       <c r="J95" t="inlineStr"/>
       <c r="K95" t="inlineStr"/>
@@ -7775,15 +7469,11 @@
       <c r="H96" t="n">
         <v>1</v>
       </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J96" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I96" t="n">
+        <v>399</v>
+      </c>
+      <c r="J96" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K96" t="inlineStr"/>
       <c r="L96" t="inlineStr">
@@ -7852,15 +7542,11 @@
       <c r="H97" t="n">
         <v>1</v>
       </c>
-      <c r="I97" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I97" t="n">
+        <v>449</v>
+      </c>
+      <c r="J97" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K97" t="inlineStr"/>
       <c r="L97" t="inlineStr">
@@ -7930,10 +7616,8 @@
         <v>1</v>
       </c>
       <c r="I98" t="inlineStr"/>
-      <c r="J98" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J98" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K98" t="inlineStr"/>
       <c r="L98" t="inlineStr">
@@ -8002,15 +7686,11 @@
       <c r="H99" t="n">
         <v>3</v>
       </c>
-      <c r="I99" t="inlineStr">
-        <is>
-          <t>1,347.00</t>
-        </is>
-      </c>
-      <c r="J99" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I99" t="n">
+        <v>1347</v>
+      </c>
+      <c r="J99" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K99" t="inlineStr"/>
       <c r="L99" t="inlineStr">
@@ -8079,15 +7759,11 @@
       <c r="H100" t="n">
         <v>1</v>
       </c>
-      <c r="I100" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J100" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I100" t="n">
+        <v>549</v>
+      </c>
+      <c r="J100" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K100" t="inlineStr"/>
       <c r="L100" t="inlineStr">
@@ -8156,10 +7832,8 @@
       <c r="H101" t="n">
         <v>1</v>
       </c>
-      <c r="I101" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
+      <c r="I101" t="n">
+        <v>399</v>
       </c>
       <c r="J101" t="inlineStr"/>
       <c r="K101" t="inlineStr">
@@ -8233,15 +7907,11 @@
       <c r="H102" t="n">
         <v>1</v>
       </c>
-      <c r="I102" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J102" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I102" t="n">
+        <v>449</v>
+      </c>
+      <c r="J102" t="n">
+        <v>60.18</v>
       </c>
       <c r="K102" t="inlineStr"/>
       <c r="L102" t="inlineStr">
@@ -8310,15 +7980,11 @@
       <c r="H103" t="n">
         <v>1</v>
       </c>
-      <c r="I103" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J103" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I103" t="n">
+        <v>549</v>
+      </c>
+      <c r="J103" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K103" t="inlineStr">
         <is>
@@ -8391,15 +8057,11 @@
       <c r="H104" t="n">
         <v>1</v>
       </c>
-      <c r="I104" t="inlineStr">
-        <is>
-          <t>499.00</t>
-        </is>
-      </c>
-      <c r="J104" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I104" t="n">
+        <v>499</v>
+      </c>
+      <c r="J104" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K104" t="inlineStr"/>
       <c r="L104" t="inlineStr">
@@ -8468,15 +8130,11 @@
       <c r="H105" t="n">
         <v>1</v>
       </c>
-      <c r="I105" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J105" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I105" t="n">
+        <v>449</v>
+      </c>
+      <c r="J105" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -8549,15 +8207,11 @@
       <c r="H106" t="n">
         <v>1</v>
       </c>
-      <c r="I106" t="inlineStr">
-        <is>
-          <t>649.00</t>
-        </is>
-      </c>
-      <c r="J106" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I106" t="n">
+        <v>649</v>
+      </c>
+      <c r="J106" t="n">
+        <v>60.18</v>
       </c>
       <c r="K106" t="inlineStr"/>
       <c r="L106" t="inlineStr">
@@ -8626,15 +8280,11 @@
       <c r="H107" t="n">
         <v>1</v>
       </c>
-      <c r="I107" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J107" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I107" t="n">
+        <v>399</v>
+      </c>
+      <c r="J107" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K107" t="inlineStr"/>
       <c r="L107" t="inlineStr">
@@ -8704,10 +8354,8 @@
         <v>1</v>
       </c>
       <c r="I108" t="inlineStr"/>
-      <c r="J108" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J108" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K108" t="inlineStr"/>
       <c r="L108" t="inlineStr">
@@ -8776,15 +8424,11 @@
       <c r="H109" t="n">
         <v>1</v>
       </c>
-      <c r="I109" t="inlineStr">
-        <is>
-          <t>475.00</t>
-        </is>
-      </c>
-      <c r="J109" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I109" t="n">
+        <v>475</v>
+      </c>
+      <c r="J109" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K109" t="inlineStr">
         <is>
@@ -8857,15 +8501,11 @@
       <c r="H110" t="n">
         <v>1</v>
       </c>
-      <c r="I110" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J110" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I110" t="n">
+        <v>399</v>
+      </c>
+      <c r="J110" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K110" t="inlineStr">
         <is>
@@ -8938,15 +8578,11 @@
       <c r="H111" t="n">
         <v>1</v>
       </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J111" t="inlineStr">
-        <is>
-          <t>80.24</t>
-        </is>
+      <c r="I111" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J111" t="n">
+        <v>80.23999999999999</v>
       </c>
       <c r="K111" t="inlineStr"/>
       <c r="L111" t="inlineStr">
@@ -9015,15 +8651,11 @@
       <c r="H112" t="n">
         <v>1</v>
       </c>
-      <c r="I112" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J112" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I112" t="n">
+        <v>449</v>
+      </c>
+      <c r="J112" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K112" t="inlineStr"/>
       <c r="L112" t="inlineStr">
@@ -9092,15 +8724,11 @@
       <c r="H113" t="n">
         <v>1</v>
       </c>
-      <c r="I113" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J113" t="inlineStr">
-        <is>
-          <t>146.32</t>
-        </is>
+      <c r="I113" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J113" t="n">
+        <v>146.32</v>
       </c>
       <c r="K113" t="inlineStr"/>
       <c r="L113" t="inlineStr">
@@ -9169,15 +8797,11 @@
       <c r="H114" t="n">
         <v>1</v>
       </c>
-      <c r="I114" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J114" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I114" t="n">
+        <v>549</v>
+      </c>
+      <c r="J114" t="n">
+        <v>60.18</v>
       </c>
       <c r="K114" t="inlineStr">
         <is>
@@ -9250,15 +8874,11 @@
       <c r="H115" t="n">
         <v>1</v>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J115" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I115" t="n">
+        <v>399</v>
+      </c>
+      <c r="J115" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K115" t="inlineStr"/>
       <c r="L115" t="inlineStr">
@@ -9328,10 +8948,8 @@
         <v>1</v>
       </c>
       <c r="I116" t="inlineStr"/>
-      <c r="J116" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J116" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K116" t="inlineStr"/>
       <c r="L116" t="inlineStr">
@@ -9401,10 +9019,8 @@
         <v>1</v>
       </c>
       <c r="I117" t="inlineStr"/>
-      <c r="J117" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J117" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K117" t="inlineStr">
         <is>
@@ -9477,15 +9093,11 @@
       <c r="H118" t="n">
         <v>1</v>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J118" t="inlineStr">
-        <is>
-          <t>114.46</t>
-        </is>
+      <c r="I118" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J118" t="n">
+        <v>114.46</v>
       </c>
       <c r="K118" t="inlineStr">
         <is>
@@ -9558,15 +9170,11 @@
       <c r="H119" t="n">
         <v>3</v>
       </c>
-      <c r="I119" t="inlineStr">
-        <is>
-          <t>3,897.00</t>
-        </is>
-      </c>
-      <c r="J119" t="inlineStr">
-        <is>
-          <t>133.34</t>
-        </is>
+      <c r="I119" t="n">
+        <v>3897</v>
+      </c>
+      <c r="J119" t="n">
+        <v>133.34</v>
       </c>
       <c r="K119" t="inlineStr"/>
       <c r="L119" t="inlineStr">
@@ -9635,15 +9243,11 @@
       <c r="H120" t="n">
         <v>1</v>
       </c>
-      <c r="I120" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J120" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I120" t="n">
+        <v>449</v>
+      </c>
+      <c r="J120" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K120" t="inlineStr"/>
       <c r="L120" t="inlineStr">
@@ -9712,15 +9316,11 @@
       <c r="H121" t="n">
         <v>1</v>
       </c>
-      <c r="I121" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J121" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I121" t="n">
+        <v>449</v>
+      </c>
+      <c r="J121" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K121" t="inlineStr"/>
       <c r="L121" t="inlineStr">
@@ -9789,15 +9389,11 @@
       <c r="H122" t="n">
         <v>1</v>
       </c>
-      <c r="I122" t="inlineStr">
-        <is>
-          <t>1,499.00</t>
-        </is>
-      </c>
-      <c r="J122" t="inlineStr">
-        <is>
-          <t>114.46</t>
-        </is>
+      <c r="I122" t="n">
+        <v>1499</v>
+      </c>
+      <c r="J122" t="n">
+        <v>114.46</v>
       </c>
       <c r="K122" t="inlineStr"/>
       <c r="L122" t="inlineStr">
@@ -9866,15 +9462,11 @@
       <c r="H123" t="n">
         <v>3</v>
       </c>
-      <c r="I123" t="inlineStr">
-        <is>
-          <t>3,897.00</t>
-        </is>
-      </c>
-      <c r="J123" t="inlineStr">
-        <is>
-          <t>241.90</t>
-        </is>
+      <c r="I123" t="n">
+        <v>3897</v>
+      </c>
+      <c r="J123" t="n">
+        <v>241.9</v>
       </c>
       <c r="K123" t="inlineStr"/>
       <c r="L123" t="inlineStr">
@@ -9943,15 +9535,11 @@
       <c r="H124" t="n">
         <v>1</v>
       </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
-      </c>
-      <c r="J124" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I124" t="n">
+        <v>349</v>
+      </c>
+      <c r="J124" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K124" t="inlineStr"/>
       <c r="L124" t="inlineStr">
@@ -10020,15 +9608,11 @@
       <c r="H125" t="n">
         <v>1</v>
       </c>
-      <c r="I125" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J125" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I125" t="n">
+        <v>449</v>
+      </c>
+      <c r="J125" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K125" t="inlineStr"/>
       <c r="L125" t="inlineStr">
@@ -10097,15 +9681,11 @@
       <c r="H126" t="n">
         <v>1</v>
       </c>
-      <c r="I126" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J126" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I126" t="n">
+        <v>449</v>
+      </c>
+      <c r="J126" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K126" t="inlineStr"/>
       <c r="L126" t="inlineStr">
@@ -10174,15 +9754,11 @@
       <c r="H127" t="n">
         <v>1</v>
       </c>
-      <c r="I127" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J127" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I127" t="n">
+        <v>399</v>
+      </c>
+      <c r="J127" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K127" t="inlineStr"/>
       <c r="L127" t="inlineStr">
@@ -10251,15 +9827,11 @@
       <c r="H128" t="n">
         <v>1</v>
       </c>
-      <c r="I128" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
-      </c>
-      <c r="J128" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I128" t="n">
+        <v>349</v>
+      </c>
+      <c r="J128" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K128" t="inlineStr"/>
       <c r="L128" t="inlineStr">
@@ -10328,15 +9900,11 @@
       <c r="H129" t="n">
         <v>1</v>
       </c>
-      <c r="I129" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J129" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I129" t="n">
+        <v>449</v>
+      </c>
+      <c r="J129" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K129" t="inlineStr"/>
       <c r="L129" t="inlineStr">
@@ -10405,15 +9973,11 @@
       <c r="H130" t="n">
         <v>1</v>
       </c>
-      <c r="I130" t="inlineStr">
-        <is>
-          <t>899.00</t>
-        </is>
-      </c>
-      <c r="J130" t="inlineStr">
-        <is>
-          <t>114.46</t>
-        </is>
+      <c r="I130" t="n">
+        <v>899</v>
+      </c>
+      <c r="J130" t="n">
+        <v>114.46</v>
       </c>
       <c r="K130" t="inlineStr"/>
       <c r="L130" t="inlineStr">
@@ -10482,15 +10046,11 @@
       <c r="H131" t="n">
         <v>1</v>
       </c>
-      <c r="I131" t="inlineStr">
-        <is>
-          <t>475.00</t>
-        </is>
-      </c>
-      <c r="J131" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I131" t="n">
+        <v>475</v>
+      </c>
+      <c r="J131" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K131" t="inlineStr"/>
       <c r="L131" t="inlineStr">
@@ -10559,15 +10119,11 @@
       <c r="H132" t="n">
         <v>1</v>
       </c>
-      <c r="I132" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J132" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I132" t="n">
+        <v>549</v>
+      </c>
+      <c r="J132" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K132" t="inlineStr"/>
       <c r="L132" t="inlineStr">
@@ -10636,15 +10192,11 @@
       <c r="H133" t="n">
         <v>1</v>
       </c>
-      <c r="I133" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J133" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I133" t="n">
+        <v>449</v>
+      </c>
+      <c r="J133" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K133" t="inlineStr"/>
       <c r="L133" t="inlineStr">
@@ -10713,15 +10265,11 @@
       <c r="H134" t="n">
         <v>1</v>
       </c>
-      <c r="I134" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J134" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I134" t="n">
+        <v>399</v>
+      </c>
+      <c r="J134" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K134" t="inlineStr"/>
       <c r="L134" t="inlineStr">
@@ -10790,15 +10338,11 @@
       <c r="H135" t="n">
         <v>1</v>
       </c>
-      <c r="I135" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J135" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I135" t="n">
+        <v>449</v>
+      </c>
+      <c r="J135" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K135" t="inlineStr"/>
       <c r="L135" t="inlineStr">
@@ -10868,10 +10412,8 @@
         <v>1</v>
       </c>
       <c r="I136" t="inlineStr"/>
-      <c r="J136" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J136" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K136" t="inlineStr"/>
       <c r="L136" t="inlineStr">
@@ -10940,15 +10482,11 @@
       <c r="H137" t="n">
         <v>1</v>
       </c>
-      <c r="I137" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J137" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I137" t="n">
+        <v>449</v>
+      </c>
+      <c r="J137" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K137" t="inlineStr">
         <is>
@@ -11021,15 +10559,11 @@
       <c r="H138" t="n">
         <v>4</v>
       </c>
-      <c r="I138" t="inlineStr">
-        <is>
-          <t>1,796.00</t>
-        </is>
-      </c>
-      <c r="J138" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I138" t="n">
+        <v>1796</v>
+      </c>
+      <c r="J138" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K138" t="inlineStr"/>
       <c r="L138" t="inlineStr">
@@ -11098,15 +10632,11 @@
       <c r="H139" t="n">
         <v>1</v>
       </c>
-      <c r="I139" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J139" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I139" t="n">
+        <v>449</v>
+      </c>
+      <c r="J139" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K139" t="inlineStr"/>
       <c r="L139" t="inlineStr">
@@ -11175,15 +10705,11 @@
       <c r="H140" t="n">
         <v>1</v>
       </c>
-      <c r="I140" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J140" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I140" t="n">
+        <v>449</v>
+      </c>
+      <c r="J140" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K140" t="inlineStr"/>
       <c r="L140" t="inlineStr">
@@ -11252,15 +10778,11 @@
       <c r="H141" t="n">
         <v>1</v>
       </c>
-      <c r="I141" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J141" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I141" t="n">
+        <v>549</v>
+      </c>
+      <c r="J141" t="n">
+        <v>47.2</v>
       </c>
       <c r="K141" t="inlineStr"/>
       <c r="L141" t="inlineStr">
@@ -11329,15 +10851,11 @@
       <c r="H142" t="n">
         <v>1</v>
       </c>
-      <c r="I142" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J142" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I142" t="n">
+        <v>399</v>
+      </c>
+      <c r="J142" t="n">
+        <v>47.2</v>
       </c>
       <c r="K142" t="inlineStr"/>
       <c r="L142" t="inlineStr">
@@ -11406,15 +10924,11 @@
       <c r="H143" t="n">
         <v>1</v>
       </c>
-      <c r="I143" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
-      </c>
-      <c r="J143" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I143" t="n">
+        <v>349</v>
+      </c>
+      <c r="J143" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K143" t="inlineStr"/>
       <c r="L143" t="inlineStr">
@@ -11483,15 +10997,11 @@
       <c r="H144" t="n">
         <v>1</v>
       </c>
-      <c r="I144" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J144" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I144" t="n">
+        <v>449</v>
+      </c>
+      <c r="J144" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K144" t="inlineStr">
         <is>
@@ -11564,15 +11074,11 @@
       <c r="H145" t="n">
         <v>1</v>
       </c>
-      <c r="I145" t="inlineStr">
-        <is>
-          <t>475.00</t>
-        </is>
-      </c>
-      <c r="J145" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I145" t="n">
+        <v>475</v>
+      </c>
+      <c r="J145" t="n">
+        <v>47.2</v>
       </c>
       <c r="K145" t="inlineStr"/>
       <c r="L145" t="inlineStr">
@@ -11641,15 +11147,11 @@
       <c r="H146" t="n">
         <v>1</v>
       </c>
-      <c r="I146" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J146" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I146" t="n">
+        <v>449</v>
+      </c>
+      <c r="J146" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K146" t="inlineStr">
         <is>
@@ -11722,15 +11224,11 @@
       <c r="H147" t="n">
         <v>1</v>
       </c>
-      <c r="I147" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
-      </c>
-      <c r="J147" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I147" t="n">
+        <v>349</v>
+      </c>
+      <c r="J147" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K147" t="inlineStr"/>
       <c r="L147" t="inlineStr">
@@ -11799,15 +11297,11 @@
       <c r="H148" t="n">
         <v>1</v>
       </c>
-      <c r="I148" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J148" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I148" t="n">
+        <v>449</v>
+      </c>
+      <c r="J148" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K148" t="inlineStr"/>
       <c r="L148" t="inlineStr">
@@ -11876,15 +11370,11 @@
       <c r="H149" t="n">
         <v>1</v>
       </c>
-      <c r="I149" t="inlineStr">
-        <is>
-          <t>475.00</t>
-        </is>
-      </c>
-      <c r="J149" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I149" t="n">
+        <v>475</v>
+      </c>
+      <c r="J149" t="n">
+        <v>60.18</v>
       </c>
       <c r="K149" t="inlineStr"/>
       <c r="L149" t="inlineStr">
@@ -11953,15 +11443,11 @@
       <c r="H150" t="n">
         <v>1</v>
       </c>
-      <c r="I150" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J150" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I150" t="n">
+        <v>399</v>
+      </c>
+      <c r="J150" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K150" t="inlineStr"/>
       <c r="L150" t="inlineStr">
@@ -12030,15 +11516,11 @@
       <c r="H151" t="n">
         <v>1</v>
       </c>
-      <c r="I151" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J151" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I151" t="n">
+        <v>449</v>
+      </c>
+      <c r="J151" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K151" t="inlineStr">
         <is>
@@ -12112,10 +11594,8 @@
         <v>1</v>
       </c>
       <c r="I152" t="inlineStr"/>
-      <c r="J152" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J152" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K152" t="inlineStr"/>
       <c r="L152" t="inlineStr">
@@ -12184,15 +11664,11 @@
       <c r="H153" t="n">
         <v>1</v>
       </c>
-      <c r="I153" t="inlineStr">
-        <is>
-          <t>349.00</t>
-        </is>
-      </c>
-      <c r="J153" t="inlineStr">
-        <is>
-          <t>60.18</t>
-        </is>
+      <c r="I153" t="n">
+        <v>349</v>
+      </c>
+      <c r="J153" t="n">
+        <v>60.18</v>
       </c>
       <c r="K153" t="inlineStr"/>
       <c r="L153" t="inlineStr">
@@ -12261,15 +11737,11 @@
       <c r="H154" t="n">
         <v>1</v>
       </c>
-      <c r="I154" t="inlineStr">
-        <is>
-          <t>549.00</t>
-        </is>
-      </c>
-      <c r="J154" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I154" t="n">
+        <v>549</v>
+      </c>
+      <c r="J154" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K154" t="inlineStr"/>
       <c r="L154" t="inlineStr">
@@ -12338,15 +11810,11 @@
       <c r="H155" t="n">
         <v>1</v>
       </c>
-      <c r="I155" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J155" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I155" t="n">
+        <v>449</v>
+      </c>
+      <c r="J155" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K155" t="inlineStr"/>
       <c r="L155" t="inlineStr">
@@ -12415,15 +11883,11 @@
       <c r="H156" t="n">
         <v>1</v>
       </c>
-      <c r="I156" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J156" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I156" t="n">
+        <v>449</v>
+      </c>
+      <c r="J156" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K156" t="inlineStr"/>
       <c r="L156" t="inlineStr">
@@ -12493,10 +11957,8 @@
         <v>1</v>
       </c>
       <c r="I157" t="inlineStr"/>
-      <c r="J157" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J157" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K157" t="inlineStr"/>
       <c r="L157" t="inlineStr">
@@ -12565,15 +12027,11 @@
       <c r="H158" t="n">
         <v>1</v>
       </c>
-      <c r="I158" t="inlineStr">
-        <is>
-          <t>475.00</t>
-        </is>
-      </c>
-      <c r="J158" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I158" t="n">
+        <v>475</v>
+      </c>
+      <c r="J158" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K158" t="inlineStr"/>
       <c r="L158" t="inlineStr">
@@ -12642,15 +12100,11 @@
       <c r="H159" t="n">
         <v>1</v>
       </c>
-      <c r="I159" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J159" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I159" t="n">
+        <v>399</v>
+      </c>
+      <c r="J159" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K159" t="inlineStr">
         <is>
@@ -12723,15 +12177,11 @@
       <c r="H160" t="n">
         <v>1</v>
       </c>
-      <c r="I160" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J160" t="inlineStr">
-        <is>
-          <t>47.20</t>
-        </is>
+      <c r="I160" t="n">
+        <v>449</v>
+      </c>
+      <c r="J160" t="n">
+        <v>47.2</v>
       </c>
       <c r="K160" t="inlineStr">
         <is>
@@ -12805,10 +12255,8 @@
         <v>1</v>
       </c>
       <c r="I161" t="inlineStr"/>
-      <c r="J161" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="J161" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K161" t="inlineStr">
         <is>
@@ -12881,15 +12329,11 @@
       <c r="H162" t="n">
         <v>1</v>
       </c>
-      <c r="I162" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J162" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I162" t="n">
+        <v>449</v>
+      </c>
+      <c r="J162" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K162" t="inlineStr"/>
       <c r="L162" t="inlineStr">
@@ -12958,15 +12402,11 @@
       <c r="H163" t="n">
         <v>1</v>
       </c>
-      <c r="I163" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J163" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I163" t="n">
+        <v>449</v>
+      </c>
+      <c r="J163" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K163" t="inlineStr"/>
       <c r="L163" t="inlineStr">
@@ -13035,15 +12475,11 @@
       <c r="H164" t="n">
         <v>1</v>
       </c>
-      <c r="I164" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J164" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I164" t="n">
+        <v>449</v>
+      </c>
+      <c r="J164" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K164" t="inlineStr"/>
       <c r="L164" t="inlineStr">
@@ -13112,15 +12548,11 @@
       <c r="H165" t="n">
         <v>1</v>
       </c>
-      <c r="I165" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J165" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I165" t="n">
+        <v>449</v>
+      </c>
+      <c r="J165" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K165" t="inlineStr">
         <is>
@@ -13193,15 +12625,11 @@
       <c r="H166" t="n">
         <v>1</v>
       </c>
-      <c r="I166" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J166" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I166" t="n">
+        <v>399</v>
+      </c>
+      <c r="J166" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K166" t="inlineStr"/>
       <c r="L166" t="inlineStr">
@@ -13270,15 +12698,11 @@
       <c r="H167" t="n">
         <v>1</v>
       </c>
-      <c r="I167" t="inlineStr">
-        <is>
-          <t>399.00</t>
-        </is>
-      </c>
-      <c r="J167" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I167" t="n">
+        <v>399</v>
+      </c>
+      <c r="J167" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K167" t="inlineStr"/>
       <c r="L167" t="inlineStr">
@@ -13347,15 +12771,11 @@
       <c r="H168" t="n">
         <v>3</v>
       </c>
-      <c r="I168" t="inlineStr">
-        <is>
-          <t>1,347.00</t>
-        </is>
-      </c>
-      <c r="J168" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I168" t="n">
+        <v>1347</v>
+      </c>
+      <c r="J168" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K168" t="inlineStr">
         <is>
@@ -13428,15 +12848,11 @@
       <c r="H169" t="n">
         <v>1</v>
       </c>
-      <c r="I169" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J169" t="inlineStr">
-        <is>
-          <t>114.46</t>
-        </is>
+      <c r="I169" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J169" t="n">
+        <v>114.46</v>
       </c>
       <c r="K169" t="inlineStr"/>
       <c r="L169" t="inlineStr">
@@ -13505,15 +12921,11 @@
       <c r="H170" t="n">
         <v>1</v>
       </c>
-      <c r="I170" t="inlineStr">
-        <is>
-          <t>1,299.00</t>
-        </is>
-      </c>
-      <c r="J170" t="inlineStr">
-        <is>
-          <t>105.02</t>
-        </is>
+      <c r="I170" t="n">
+        <v>1299</v>
+      </c>
+      <c r="J170" t="n">
+        <v>105.02</v>
       </c>
       <c r="K170" t="inlineStr"/>
       <c r="L170" t="inlineStr">
@@ -13582,15 +12994,11 @@
       <c r="H171" t="n">
         <v>1</v>
       </c>
-      <c r="I171" t="inlineStr">
-        <is>
-          <t>1,499.00</t>
-        </is>
-      </c>
-      <c r="J171" t="inlineStr">
-        <is>
-          <t>80.24</t>
-        </is>
+      <c r="I171" t="n">
+        <v>1499</v>
+      </c>
+      <c r="J171" t="n">
+        <v>80.23999999999999</v>
       </c>
       <c r="K171" t="inlineStr">
         <is>
@@ -13663,15 +13071,11 @@
       <c r="H172" t="n">
         <v>1</v>
       </c>
-      <c r="I172" t="inlineStr">
-        <is>
-          <t>449.00</t>
-        </is>
-      </c>
-      <c r="J172" t="inlineStr">
-        <is>
-          <t>84.96</t>
-        </is>
+      <c r="I172" t="n">
+        <v>449</v>
+      </c>
+      <c r="J172" t="n">
+        <v>84.95999999999999</v>
       </c>
       <c r="K172" t="inlineStr"/>
       <c r="L172" t="inlineStr">

</xml_diff>